<commit_message>
update 29/01 y E. Gomez
</commit_message>
<xml_diff>
--- a/ec_2025_faro/xlsx/gasto_por_partido_all.xlsx
+++ b/ec_2025_faro/xlsx/gasto_por_partido_all.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>28557.5</v>
+        <v>28657.5</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>75788.5</v>
+        <v>76288.5</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1798744.63</v>
+        <v>1939273.94</v>
       </c>
     </row>
     <row r="5">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>40596.19</v>
+        <v>42501.96</v>
       </c>
     </row>
     <row r="9">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>118326.39</v>
+        <v>131397.38</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3981.22</v>
+        <v>3982.96</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>93667.05</v>
+        <v>106462.84</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3755.29</v>
+        <v>3790.84</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1980</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6435</v>
+        <v>7030</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>10868.17</v>
+        <v>11551.69</v>
       </c>
     </row>
     <row r="17">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19484.5</v>
+        <v>19984</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>14502.5</v>
+        <v>15001</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>42231.42</v>
+        <v>45878.86</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>74.37</v>
+        <v>75.06999999999999</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>12233.3</v>
+        <v>13518.67</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>508.56</v>
+        <v>513.62</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2725.95</v>
+        <v>3019.44</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>12.6</v>
+        <v>13.04</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1293</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="27">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1293</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="28">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>113540.45</v>
+        <v>124387.95</v>
       </c>
     </row>
     <row r="29">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>104506.54</v>
+        <v>114963.25</v>
       </c>
     </row>
     <row r="31">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>39046.5</v>
+        <v>39096</v>
       </c>
     </row>
     <row r="33">
@@ -927,7 +927,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>48267.5</v>
+        <v>48317</v>
       </c>
     </row>
     <row r="34">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9717.91</v>
+        <v>10514.3</v>
       </c>
     </row>
     <row r="35">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>288.95</v>
+        <v>291.07</v>
       </c>
     </row>
     <row r="36">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1096.49</v>
+        <v>1178.13</v>
       </c>
     </row>
     <row r="37">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>318003.56</v>
+        <v>344446.52</v>
       </c>
     </row>
     <row r="39">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>125723</v>
+        <v>146066.5</v>
       </c>
     </row>
     <row r="43">
@@ -1083,7 +1083,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>(SUMA) - W. Gómez - I. Díaz</t>
+          <t>(SUMA) - E. Gómez - I. Díaz</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>872.2</v>
+        <v>977.22</v>
       </c>
     </row>
     <row r="45">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2235</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="46">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2235</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="47">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>18609.37</v>
+        <v>20018.16</v>
       </c>
     </row>
     <row r="48">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>100634.5</v>
+        <v>102078.5</v>
       </c>
     </row>
     <row r="50">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>158941.5</v>
+        <v>161181.5</v>
       </c>
     </row>
     <row r="51">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2811462.62</v>
+        <v>3056156.81</v>
       </c>
     </row>
     <row r="52">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>276960.19</v>
+        <v>277005.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>